<commit_message>
remove guide_strand column and Mus musculus [GRCm38] genome from the list of possible genome as it is not yet implemented, only works now with Homo sapiens [GRCh38]
</commit_message>
<xml_diff>
--- a/data/submission_spreadsheets/SRP199742_SLX15025_GEP00010.xlsx
+++ b/data/submission_spreadsheets/SRP199742_SLX15025_GEP00010.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="21721"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="0" windowWidth="27840" windowHeight="16680" tabRatio="736" activeTab="1"/>
+    <workbookView xWindow="960" yWindow="8980" windowWidth="27840" windowHeight="8440" tabRatio="736" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="10" r:id="rId1"/>
@@ -2902,23 +2902,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -3482,6 +3465,23 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -5084,38 +5084,38 @@
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="N1:P9" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <tableColumns count="3">
-    <tableColumn id="3" name="refseq_orientation_match" dataDxfId="0"/>
-    <tableColumn id="1" name="score" dataDxfId="45"/>
-    <tableColumn id="2" name="description" dataDxfId="44"/>
+    <tableColumn id="3" name="refseq_orientation_match" dataDxfId="45"/>
+    <tableColumn id="1" name="score" dataDxfId="44"/>
+    <tableColumn id="2" name="description" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="A1:C97" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="A1:C97" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <tableColumns count="3">
-    <tableColumn id="1" name="layout_id" dataDxfId="41"/>
-    <tableColumn id="2" name="well_position" dataDxfId="40"/>
-    <tableColumn id="13" name="sequencing_barcode" dataDxfId="39"/>
+    <tableColumn id="1" name="layout_id" dataDxfId="40"/>
+    <tableColumn id="2" name="well_position" dataDxfId="39"/>
+    <tableColumn id="13" name="sequencing_barcode" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="D1:M97" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="D1:M97" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <tableColumns count="10">
-    <tableColumn id="1" name="sequencing_sample_name" dataDxfId="36"/>
-    <tableColumn id="2" name="sequencing_dna_source" dataDxfId="35"/>
-    <tableColumn id="3" name="sequencing_library_type" dataDxfId="34"/>
-    <tableColumn id="4" name="sequencing_project_id" dataDxfId="33"/>
-    <tableColumn id="5" name="cell_line_name" dataDxfId="32"/>
-    <tableColumn id="6" name="cell_pool" dataDxfId="31"/>
-    <tableColumn id="7" name="clone_name" dataDxfId="30"/>
-    <tableColumn id="8" name="content_type" dataDxfId="29"/>
-    <tableColumn id="9" name="is_control" dataDxfId="28"/>
-    <tableColumn id="10" name="replicate_group" dataDxfId="27"/>
+    <tableColumn id="1" name="sequencing_sample_name" dataDxfId="35"/>
+    <tableColumn id="2" name="sequencing_dna_source" dataDxfId="34"/>
+    <tableColumn id="3" name="sequencing_library_type" dataDxfId="33"/>
+    <tableColumn id="4" name="sequencing_project_id" dataDxfId="32"/>
+    <tableColumn id="5" name="cell_line_name" dataDxfId="31"/>
+    <tableColumn id="6" name="cell_pool" dataDxfId="30"/>
+    <tableColumn id="7" name="clone_name" dataDxfId="29"/>
+    <tableColumn id="8" name="content_type" dataDxfId="28"/>
+    <tableColumn id="9" name="is_control" dataDxfId="27"/>
+    <tableColumn id="10" name="replicate_group" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5133,50 +5133,50 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="51" name="Table51" displayName="Table51" ref="A1:D10" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="51" name="Table51" displayName="Table51" ref="A1:D10" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <tableColumns count="4">
-    <tableColumn id="1" name="layout_id" dataDxfId="24"/>
-    <tableColumn id="2" name="plate_name" dataDxfId="23"/>
-    <tableColumn id="5" name="plate_barcode" dataDxfId="22"/>
-    <tableColumn id="4" name="plate_description" dataDxfId="21"/>
+    <tableColumn id="1" name="layout_id" dataDxfId="23"/>
+    <tableColumn id="2" name="plate_name" dataDxfId="22"/>
+    <tableColumn id="5" name="plate_barcode" dataDxfId="21"/>
+    <tableColumn id="4" name="plate_description" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="A1:D19" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="A1:D19" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <tableColumns count="4">
-    <tableColumn id="1" name="guide_name" dataDxfId="18"/>
-    <tableColumn id="2" name="is_off_target_coding_region" dataDxfId="17"/>
-    <tableColumn id="3" name="number_of_mismatches" dataDxfId="16"/>
-    <tableColumn id="4" name="number_of_off_targets" dataDxfId="15"/>
+    <tableColumn id="1" name="guide_name" dataDxfId="17"/>
+    <tableColumn id="2" name="is_off_target_coding_region" dataDxfId="16"/>
+    <tableColumn id="3" name="number_of_mismatches" dataDxfId="15"/>
+    <tableColumn id="4" name="number_of_off_targets" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table119" displayName="Table119" ref="A1:C14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table119" displayName="Table119" ref="A1:C14" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="3">
-    <tableColumn id="4" name="amplicon_name" dataDxfId="12" dataCellStyle="Normal"/>
-    <tableColumn id="1" name="sequence_name" dataDxfId="11" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="sequence" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="amplicon_name" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="sequence_name" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="sequence" dataDxfId="9" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <tableColumns count="7">
-    <tableColumn id="1" name="target_genome" dataDxfId="7"/>
-    <tableColumn id="2" name="strand" dataDxfId="6"/>
-    <tableColumn id="3" name="dna_feature" dataDxfId="5"/>
-    <tableColumn id="4" name="is_true_or_false" dataDxfId="4"/>
-    <tableColumn id="5" name="experiment_type" dataDxfId="3"/>
-    <tableColumn id="6" name="content_type" dataDxfId="2"/>
-    <tableColumn id="7" name="sequencing_dna_source" dataDxfId="1"/>
+    <tableColumn id="1" name="target_genome" dataDxfId="6"/>
+    <tableColumn id="2" name="strand" dataDxfId="5"/>
+    <tableColumn id="3" name="dna_feature" dataDxfId="4"/>
+    <tableColumn id="4" name="is_true_or_false" dataDxfId="3"/>
+    <tableColumn id="5" name="experiment_type" dataDxfId="2"/>
+    <tableColumn id="6" name="content_type" dataDxfId="1"/>
+    <tableColumn id="7" name="sequencing_dna_source" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>